<commit_message>
Working with Dataframe Operations
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Python\Pyspark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2608E3F-4BAF-48DD-A595-950620A6CB68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7266281A-CFDF-4EBF-A9DB-E0DB3AD0ABA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{45CD08D4-927A-4323-BD4E-1ED4C21E5BD9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -49,6 +49,18 @@
   </si>
   <si>
     <t>Experience</t>
+  </si>
+  <si>
+    <t>Hajra</t>
+  </si>
+  <si>
+    <t>Nashra</t>
+  </si>
+  <si>
+    <t>Zainab</t>
+  </si>
+  <si>
+    <t>Salary</t>
   </si>
 </sst>
 </file>
@@ -400,15 +412,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DAA5F1-2871-4386-9E64-599B62E6C6B4}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H10" sqref="H7:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -418,8 +430,11 @@
       <c r="C1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -429,8 +444,11 @@
       <c r="C2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -441,18 +459,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>30</v>
-      </c>
       <c r="C4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -462,8 +480,11 @@
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -472,6 +493,49 @@
       </c>
       <c r="C6">
         <v>0</v>
+      </c>
+      <c r="D6">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>36</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>3500000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filter Operation with Pyspark
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Python\Pyspark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7266281A-CFDF-4EBF-A9DB-E0DB3AD0ABA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261E0973-1C7A-4FC4-B595-C2E9E108CD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{45CD08D4-927A-4323-BD4E-1ED4C21E5BD9}"/>
   </bookViews>
@@ -412,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DAA5F1-2871-4386-9E64-599B62E6C6B4}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H7:I10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,11 +458,17 @@
       <c r="C3">
         <v>5</v>
       </c>
+      <c r="D3">
+        <v>800000</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4">
+        <v>33</v>
+      </c>
       <c r="C4">
         <v>10</v>
       </c>
@@ -492,7 +498,7 @@
         <v>20</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>500000</v>
@@ -505,6 +511,9 @@
       <c r="B7">
         <v>24</v>
       </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
       <c r="D7">
         <v>450000</v>
       </c>
@@ -516,26 +525,25 @@
       <c r="B8">
         <v>2</v>
       </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10">
-        <v>36</v>
-      </c>
-      <c r="C10">
-        <v>10</v>
-      </c>
-      <c r="D10">
-        <v>3500000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11">
-        <v>38</v>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>